<commit_message>
forever start bin\www on_1_34.json
</commit_message>
<xml_diff>
--- a/templates/valet_delivery_note.xlsx
+++ b/templates/valet_delivery_note.xlsx
@@ -752,8 +752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AM33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
few delivery note changes
</commit_message>
<xml_diff>
--- a/templates/valet_delivery_note.xlsx
+++ b/templates/valet_delivery_note.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="405" windowWidth="27555" windowHeight="12300"/>
+    <workbookView xWindow="720" yWindow="465" windowWidth="27555" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$31</definedName>
+  </definedNames>
   <calcPr calcId="144525" calcOnSave="0" concurrentCalc="0"/>
 </workbook>
 </file>
@@ -105,9 +108,6 @@
     <t>${table:order.amount}</t>
   </si>
   <si>
-    <t>Всего товаров:</t>
-  </si>
-  <si>
     <t>${total_count}</t>
   </si>
   <si>
@@ -117,15 +117,9 @@
     <t>${total_amount}</t>
   </si>
   <si>
-    <t>Общество с ограниченной ответственностью «СМАРТ МАРКЕТ»</t>
-  </si>
-  <si>
     <t>тел.+7 (495) 134-39-12</t>
   </si>
   <si>
-    <t>Товарная накладная к заказу № ${order_id} от ${order_datetime}</t>
-  </si>
-  <si>
     <t>valet24.ru</t>
   </si>
   <si>
@@ -160,6 +154,15 @@
   </si>
   <si>
     <t>${gatecode}</t>
+  </si>
+  <si>
+    <t>Всего позиций:</t>
+  </si>
+  <si>
+    <t>ООО «СМАРТ МАРКЕТ»</t>
+  </si>
+  <si>
+    <t>Сопроводительный лист к заказу № ${order_id} от ${order_datetime}</t>
   </si>
 </sst>
 </file>
@@ -170,7 +173,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +285,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -308,7 +319,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -342,6 +353,39 @@
     </border>
     <border>
       <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -350,11 +394,20 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -368,7 +421,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -389,12 +442,6 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -403,15 +450,6 @@
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -446,6 +484,48 @@
     <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="1" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,16 +535,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -481,6 +552,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>247651</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="95250" y="28576"/>
+          <a:ext cx="676276" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -770,69 +890,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-    </row>
-    <row r="2" spans="1:11" s="20" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-    </row>
-    <row r="3" spans="1:11" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:11" s="20" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" spans="1:11" s="15" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="37"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+    </row>
+    <row r="3" spans="1:11" s="15" customFormat="1" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:11" s="15" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="25"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -841,26 +960,26 @@
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:11" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="3"/>
       <c r="C7" s="5"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:11" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="3"/>
       <c r="C8" s="6"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="3" t="s">
         <v>2</v>
       </c>
@@ -873,10 +992,10 @@
       <c r="E9" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
@@ -887,12 +1006,12 @@
         <v>8</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>44</v>
+      </c>
+      <c r="F10" s="26"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -905,10 +1024,10 @@
       <c r="E11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="26"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="3"/>
       <c r="C12" s="5"/>
       <c r="D12" s="3" t="s">
@@ -917,10 +1036,10 @@
       <c r="E12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="26"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="3" t="s">
         <v>15</v>
       </c>
@@ -929,34 +1048,34 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="F13" s="26"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="30"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="F14" s="26"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="26"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+      <c r="A16" s="31"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="28"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -967,191 +1086,183 @@
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="16" t="s">
+      <c r="A18" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="16" t="s">
+      <c r="C18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E18" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="F18" s="13" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+    <row r="19" spans="1:14" ht="51" x14ac:dyDescent="0.25">
+      <c r="A19" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B19" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C19" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D19" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E19" s="34" t="s">
         <v>27</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F19" s="34" t="s">
         <v>28</v>
       </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="7"/>
+      <c r="C21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="8"/>
+    </row>
+    <row r="23" spans="1:14" ht="9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>40</v>
-      </c>
+      <c r="C23" s="1"/>
+      <c r="D23" s="8"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="10"/>
-    </row>
-    <row r="24" spans="1:14" ht="9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="10"/>
+      <c r="C24" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>38</v>
+      </c>
       <c r="E24" s="1"/>
-      <c r="F24" s="10"/>
-    </row>
-    <row r="25" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="41"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="8"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="20"/>
+    </row>
+    <row r="28" spans="1:14" s="22" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="39"/>
+      <c r="C28" s="39"/>
+      <c r="D28" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="D25" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="1"/>
-      <c r="F25" s="10"/>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="10"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="34" t="s">
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="20"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="1"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="10"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="25"/>
-    </row>
-    <row r="29" spans="1:14" s="27" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="31" t="s">
-        <v>45</v>
-      </c>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="25"/>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="1"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="9"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="11"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A29:C29"/>
-    <mergeCell ref="D29:F29"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A27:F27"/>
+  <mergeCells count="5">
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="D28:F28"/>
+    <mergeCell ref="A26:F26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>